<commit_message>
fixed some bugs and add some features
</commit_message>
<xml_diff>
--- a/files/source/grade_example.xlsx
+++ b/files/source/grade_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Materials\cqes4cs\files\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\cqes4cs\files\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E38136D-EE99-4DD5-A125-C392CF2AEC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A057546D-AC14-49BC-A5B6-E204028F8554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,17 +75,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -403,17 +403,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:J20"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -433,9 +433,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
-        <v>51214108033</v>
+        <v>10000000001</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -453,9 +453,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>51214108034</v>
+        <v>10000000002</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -473,9 +473,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>51214108035</v>
+        <v>10000000003</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -493,9 +493,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>51214108036</v>
+        <v>10000000004</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -513,9 +513,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>51214108037</v>
+        <v>10000000005</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>

</xml_diff>